<commit_message>
Updated model for mowing platform, continued work on frame. Modelled battery.
</commit_message>
<xml_diff>
--- a/mechanical/development/platform/research/motor_calcs.xlsx
+++ b/mechanical/development/platform/research/motor_calcs.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="45">
   <si>
     <t>bold = input value</t>
   </si>
@@ -138,13 +138,34 @@
   </si>
   <si>
     <t>Nm</t>
+  </si>
+  <si>
+    <t>Sideways on 30 degree slope:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mass: </t>
+  </si>
+  <si>
+    <t>kg</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>Sum Moments about wheel origin:</t>
+  </si>
+  <si>
+    <t>Required Torque</t>
+  </si>
+  <si>
+    <t>force on 30 degree grade</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -174,6 +195,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -224,15 +252,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -616,280 +645,332 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:H18"/>
+  <dimension ref="B2:H24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:F12"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="2"/>
-    <col min="2" max="2" width="34" style="2"/>
-    <col min="3" max="1026" width="8.5703125" style="2"/>
-    <col min="1027" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="1" width="9.140625" style="3"/>
+    <col min="2" max="2" width="34" style="3"/>
+    <col min="3" max="1026" width="8.5703125" style="3"/>
+    <col min="1027" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="5">
+      <c r="C3" s="2">
         <f>E3*0.0254</f>
         <v>0.127</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="3">
+      <c r="E3" s="1">
         <v>5</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="F3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="G3" s="2">
+      <c r="G3" s="3">
         <f>E3*2</f>
         <v>10</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="H3" s="3" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="5">
+      <c r="C4" s="2">
         <f>E4*1.60934</f>
         <v>6.43736</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E4" s="1">
         <v>4</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="F4" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="6">
+      <c r="C5" s="4">
         <f>E5*2*PI()</f>
         <v>14.08</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="6">
+      <c r="E5" s="4">
         <f>E4*17.6/(PI()*E3*2)</f>
         <v>2.2409015987338865</v>
       </c>
-      <c r="F5" s="5" t="s">
+      <c r="F5" s="2" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B6" s="5"/>
-      <c r="C6" s="7"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="6">
+      <c r="B6" s="2"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="4">
         <f>E5*60</f>
         <v>134.4540959240332</v>
       </c>
-      <c r="F6" s="5" t="s">
+      <c r="F6" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="7"/>
-      <c r="D7" s="7"/>
-      <c r="E7" s="3">
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="1">
         <v>10</v>
       </c>
-      <c r="F7" s="5" t="s">
+      <c r="F7" s="2" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="5">
+      <c r="C8" s="2">
         <f>E8*9.81</f>
         <v>0.98100000000000009</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="D8" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="E8" s="3">
+      <c r="E8" s="1">
         <v>0.1</v>
       </c>
-      <c r="F8" s="5" t="s">
+      <c r="F8" s="2" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C9" s="5">
+      <c r="C9" s="2">
         <f>E9*0.453592</f>
         <v>54.431039999999996</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="D9" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="E9" s="3">
+      <c r="E9" s="1">
         <v>120</v>
       </c>
-      <c r="F9" s="5" t="s">
+      <c r="F9" s="2" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C10" s="5">
+      <c r="C10" s="2">
         <f>(SIN(E7*PI()/180)*9.81+C8)*C9</f>
         <v>146.11950761329993</v>
       </c>
-      <c r="D10" s="5" t="s">
+      <c r="D10" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="E10" s="5">
+      <c r="E10" s="2">
         <f>C10*0.224809</f>
         <v>32.848980387038345</v>
       </c>
-      <c r="F10" s="5" t="s">
+      <c r="F10" s="2" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C11" s="6">
+      <c r="C11" s="4">
         <f>C10/2*(C3)</f>
         <v>9.2785887334445452</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="D11" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E11" s="6">
+      <c r="E11" s="4">
         <f>E10/2*E3</f>
         <v>82.122450967595867</v>
       </c>
-      <c r="F11" s="5" t="s">
+      <c r="F11" s="2" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B12" s="5"/>
-      <c r="C12" s="6">
+      <c r="B12" s="2"/>
+      <c r="C12" s="4">
         <f>C11*10.2</f>
         <v>94.641605081134358</v>
       </c>
-      <c r="D12" s="5" t="s">
+      <c r="D12" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="E12" s="6">
+      <c r="E12" s="4">
         <f>E11*16</f>
         <v>1313.9592154815339</v>
       </c>
-      <c r="F12" s="5" t="s">
+      <c r="F12" s="2" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B14" s="4" t="s">
+      <c r="B14" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="C14" s="2">
+      <c r="C14" s="3">
         <f>C11*C5</f>
         <v>130.6425293668992</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="D14" s="3" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B16" s="2" t="s">
+      <c r="B16" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C16" s="2">
+      <c r="C16" s="3">
         <v>160</v>
       </c>
-      <c r="D16" s="2" t="s">
+      <c r="D16" s="3" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B17" s="2" t="s">
+      <c r="B17" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C17" s="1">
+      <c r="C17" s="7">
         <v>120</v>
       </c>
-      <c r="D17" s="1">
+      <c r="D17" s="7">
         <v>100</v>
       </c>
-      <c r="E17" s="1">
+      <c r="E17" s="7">
         <v>80</v>
       </c>
-      <c r="F17" s="1">
+      <c r="F17" s="7">
         <v>60</v>
       </c>
-      <c r="G17" s="2" t="s">
+      <c r="G17" s="3" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B18" s="2" t="s">
+      <c r="B18" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="C18" s="1">
+      <c r="C18" s="7">
         <v>12.73</v>
       </c>
-      <c r="D18" s="1">
+      <c r="D18" s="7">
         <v>15.28</v>
       </c>
-      <c r="E18" s="1">
+      <c r="E18" s="7">
         <v>19.100000000000001</v>
       </c>
-      <c r="F18" s="1">
+      <c r="F18" s="7">
         <v>25.46</v>
       </c>
-      <c r="G18" s="2" t="s">
+      <c r="G18" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B20" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B21" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C21" s="3">
+        <v>50</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B22" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="C22" s="3">
+        <f>C21*9.81*0.5</f>
+        <v>245.25</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B23" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C23" s="3">
+        <f>(C22*0.362)/2/0.265</f>
+        <v>167.51037735849056</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B24" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C24" s="3">
+        <f>C23*C3</f>
+        <v>21.273817924528302</v>
+      </c>
+      <c r="D24" s="3" t="s">
         <v>37</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Frame improvements, battery mounting.
</commit_message>
<xml_diff>
--- a/mechanical/development/platform/research/motor_calcs.xlsx
+++ b/mechanical/development/platform/research/motor_calcs.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="48">
   <si>
     <t>bold = input value</t>
   </si>
@@ -159,6 +159,15 @@
   </si>
   <si>
     <t>force on 30 degree grade</t>
+  </si>
+  <si>
+    <t>Angle:</t>
+  </si>
+  <si>
+    <t>wheel base distance</t>
+  </si>
+  <si>
+    <t>weight distance</t>
   </si>
 </sst>
 </file>
@@ -252,7 +261,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -262,6 +271,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -645,9 +655,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:H24"/>
+  <dimension ref="B2:H27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
@@ -927,45 +937,69 @@
         <v>39</v>
       </c>
       <c r="C21" s="3">
-        <v>50</v>
+        <v>63</v>
       </c>
       <c r="D21" s="3" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B22" s="8" t="s">
+      <c r="B22" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="C22" s="9">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B23" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="C22" s="3">
-        <f>C21*9.81*0.5</f>
-        <v>245.25</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B23" s="3" t="s">
-        <v>42</v>
-      </c>
       <c r="C23" s="3">
-        <f>(C22*0.362)/2/0.265</f>
-        <v>167.51037735849056</v>
+        <f>C21*9.81*SIN(C22*PI()/180)</f>
+        <v>309.01499999999999</v>
       </c>
       <c r="D23" s="3" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B24" s="3" t="s">
+      <c r="B24" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="C24" s="3">
+        <v>0.56799999999999995</v>
+      </c>
+    </row>
+    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B25" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="C25" s="9">
+        <v>0.15950880000000001</v>
+      </c>
+    </row>
+    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B26" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C26" s="3">
+        <f>(C23*C25)/2/(C24/2)</f>
+        <v>86.779246183098593</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B27" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="C24" s="3">
-        <f>C23*C3</f>
-        <v>21.273817924528302</v>
-      </c>
-      <c r="D24" s="3" t="s">
+      <c r="C27" s="3">
+        <f>C26*C3</f>
+        <v>11.020964265253522</v>
+      </c>
+      <c r="D27" s="3" t="s">
         <v>37</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Electrical panel layout work.
</commit_message>
<xml_diff>
--- a/mechanical/development/platform/research/motor_calcs.xlsx
+++ b/mechanical/development/platform/research/motor_calcs.xlsx
@@ -261,7 +261,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -271,7 +271,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -944,10 +943,10 @@
       </c>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B22" s="9" t="s">
+      <c r="B22" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="C22" s="9">
+      <c r="C22" s="3">
         <v>30</v>
       </c>
     </row>
@@ -975,8 +974,8 @@
       <c r="B25" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="C25" s="9">
-        <v>0.15950880000000001</v>
+      <c r="C25" s="3">
+        <v>0.14399999999999999</v>
       </c>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.25">
@@ -985,7 +984,7 @@
       </c>
       <c r="C26" s="3">
         <f>(C23*C25)/2/(C24/2)</f>
-        <v>86.779246183098593</v>
+        <v>78.341830985915479</v>
       </c>
       <c r="D26" s="3" t="s">
         <v>41</v>
@@ -997,7 +996,7 @@
       </c>
       <c r="C27" s="3">
         <f>C26*C3</f>
-        <v>11.020964265253522</v>
+        <v>9.9494125352112661</v>
       </c>
       <c r="D27" s="3" t="s">
         <v>37</v>

</xml_diff>

<commit_message>
Finalizing BOM, altering alignment of components. Added stand for Zed camera.
</commit_message>
<xml_diff>
--- a/mechanical/development/platform/research/motor_calcs.xlsx
+++ b/mechanical/development/platform/research/motor_calcs.xlsx
@@ -656,7 +656,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:H27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
@@ -936,7 +936,7 @@
         <v>39</v>
       </c>
       <c r="C21" s="3">
-        <v>63</v>
+        <v>50</v>
       </c>
       <c r="D21" s="3" t="s">
         <v>40</v>
@@ -956,7 +956,7 @@
       </c>
       <c r="C23" s="3">
         <f>C21*9.81*SIN(C22*PI()/180)</f>
-        <v>309.01499999999999</v>
+        <v>245.24999999999997</v>
       </c>
       <c r="D23" s="3" t="s">
         <v>41</v>
@@ -975,7 +975,7 @@
         <v>47</v>
       </c>
       <c r="C25" s="3">
-        <v>0.14399999999999999</v>
+        <v>0.13</v>
       </c>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.25">
@@ -984,7 +984,7 @@
       </c>
       <c r="C26" s="3">
         <f>(C23*C25)/2/(C24/2)</f>
-        <v>78.341830985915479</v>
+        <v>56.131161971830984</v>
       </c>
       <c r="D26" s="3" t="s">
         <v>41</v>
@@ -996,7 +996,7 @@
       </c>
       <c r="C27" s="3">
         <f>C26*C3</f>
-        <v>9.9494125352112661</v>
+        <v>7.1286575704225354</v>
       </c>
       <c r="D27" s="3" t="s">
         <v>37</v>

</xml_diff>

<commit_message>
Updated CAD files for bumblebee location. adding various media files.
</commit_message>
<xml_diff>
--- a/mechanical/development/platform/research/motor_calcs.xlsx
+++ b/mechanical/development/platform/research/motor_calcs.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18625"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="50">
   <si>
     <t>bold = input value</t>
   </si>
@@ -168,6 +168,12 @@
   </si>
   <si>
     <t>weight distance</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>deg</t>
   </si>
 </sst>
 </file>
@@ -261,7 +267,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -270,7 +276,9 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -656,8 +664,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:H27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20:D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -927,38 +935,41 @@
       </c>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B20" s="3" t="s">
+      <c r="B20" s="2" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B21" s="3" t="s">
+      <c r="B21" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C21" s="3">
+      <c r="C21" s="2">
         <v>50</v>
       </c>
-      <c r="D21" s="3" t="s">
+      <c r="D21" s="9" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B22" s="3" t="s">
+      <c r="B22" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="C22" s="3">
+      <c r="C22" s="2">
         <v>30</v>
+      </c>
+      <c r="D22" s="9" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B23" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="C23" s="3">
+      <c r="C23" s="2">
         <f>C21*9.81*SIN(C22*PI()/180)</f>
         <v>245.24999999999997</v>
       </c>
-      <c r="D23" s="3" t="s">
+      <c r="D23" s="2" t="s">
         <v>41</v>
       </c>
     </row>
@@ -966,39 +977,45 @@
       <c r="B24" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="C24" s="3">
+      <c r="C24" s="2">
         <v>0.56799999999999995</v>
+      </c>
+      <c r="D24" s="9" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B25" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="C25" s="3">
+      <c r="C25" s="2">
         <v>0.13</v>
       </c>
+      <c r="D25" s="10" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B26" s="3" t="s">
+      <c r="B26" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C26" s="3">
+      <c r="C26" s="2">
         <f>(C23*C25)/2/(C24/2)</f>
         <v>56.131161971830984</v>
       </c>
-      <c r="D26" s="3" t="s">
+      <c r="D26" s="2" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B27" s="3" t="s">
+      <c r="B27" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="C27" s="3">
+      <c r="C27" s="2">
         <f>C26*C3</f>
         <v>7.1286575704225354</v>
       </c>
-      <c r="D27" s="3" t="s">
+      <c r="D27" s="2" t="s">
         <v>37</v>
       </c>
     </row>

</xml_diff>